<commit_message>
Checking the commit by updating the attendance
</commit_message>
<xml_diff>
--- a/attendance_data.xlsx
+++ b/attendance_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\attendance_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941FFF0C-526C-4D53-B6B3-C181E5CB012F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0900DB78-E177-43D5-A1A1-C4E868AFBE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F33DA19-6151-4346-A3A3-5311E8A75F56}"/>
   </bookViews>
@@ -1550,7 +1550,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="D4" s="11">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>7</v>
@@ -1719,7 +1719,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>90</v>
@@ -1728,18 +1728,18 @@
         <v>89</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K4" s="8">
         <v>5</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M4" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O4" s="2"/>
     </row>

</xml_diff>

<commit_message>
Just attendance updates thatsit
</commit_message>
<xml_diff>
--- a/attendance_data.xlsx
+++ b/attendance_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\attendance_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B36F06-41DC-4F76-8130-318FC1E55C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BA789B-FFB4-471A-967F-275E582BA360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F33DA19-6151-4346-A3A3-5311E8A75F56}"/>
   </bookViews>
@@ -1163,7 +1163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1214,9 +1214,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1538,7 +1535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N8" sqref="N8"/>
+      <selection pane="topRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1603,7 +1600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30">
+    <row r="2" spans="1:17" ht="15.6">
       <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
@@ -1654,7 +1651,7 @@
       </c>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="30">
+    <row r="3" spans="1:17" ht="15.6">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -1705,7 +1702,7 @@
       </c>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="30">
+    <row r="4" spans="1:17" ht="15.6">
       <c r="A4" s="6" t="s">
         <v>105</v>
       </c>
@@ -1756,7 +1753,7 @@
       </c>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="30">
+    <row r="5" spans="1:17" ht="15.6">
       <c r="A5" s="6" t="s">
         <v>104</v>
       </c>
@@ -1807,7 +1804,7 @@
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" ht="30">
+    <row r="6" spans="1:17" ht="15.6">
       <c r="A6" s="10" t="s">
         <v>107</v>
       </c>
@@ -1858,7 +1855,7 @@
       </c>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="30">
+    <row r="7" spans="1:17" ht="15.6">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
@@ -1909,7 +1906,7 @@
       </c>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30">
+    <row r="8" spans="1:17" ht="15.6">
       <c r="A8" s="10" t="s">
         <v>106</v>
       </c>
@@ -1960,7 +1957,7 @@
       </c>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30">
+    <row r="9" spans="1:17" ht="15.6">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -1996,7 +1993,7 @@
         <v>89</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M9" s="10">
         <v>5</v>
@@ -2010,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="30">
+    <row r="10" spans="1:17" ht="15.6">
       <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
@@ -2060,7 +2057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="30">
+    <row r="11" spans="1:17" ht="15.6">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -2110,7 +2107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30">
+    <row r="12" spans="1:17" ht="15.6">
       <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
@@ -2160,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="30">
+    <row r="13" spans="1:17" ht="15.6">
       <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
@@ -2210,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="30">
+    <row r="14" spans="1:17" ht="15.6">
       <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
@@ -2260,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="30">
+    <row r="15" spans="1:17" ht="15.6">
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
@@ -2310,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="30">
+    <row r="16" spans="1:17" ht="15.6">
       <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
@@ -2360,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30">
+    <row r="17" spans="1:15" ht="15.6">
       <c r="A17" s="6" t="s">
         <v>94</v>
       </c>
@@ -2410,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30">
+    <row r="18" spans="1:15" ht="15.6">
       <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
@@ -2460,7 +2457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="30">
+    <row r="19" spans="1:15" ht="15.6">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
@@ -2510,7 +2507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="30">
+    <row r="20" spans="1:15" ht="15.6">
       <c r="A20" s="6" t="s">
         <v>92</v>
       </c>
@@ -2560,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="30">
+    <row r="21" spans="1:15" ht="15.6">
       <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
@@ -2610,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="30">
+    <row r="22" spans="1:15" ht="15.6">
       <c r="A22" s="6" t="s">
         <v>95</v>
       </c>
@@ -2660,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="30">
+    <row r="23" spans="1:15" ht="15.6">
       <c r="A23" s="10" t="s">
         <v>19</v>
       </c>
@@ -2710,7 +2707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30">
+    <row r="24" spans="1:15" ht="15.6">
       <c r="A24" s="10" t="s">
         <v>108</v>
       </c>
@@ -2760,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="30">
+    <row r="25" spans="1:15" ht="15.6">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -2810,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30">
+    <row r="26" spans="1:15" ht="15.6">
       <c r="A26" s="6" t="s">
         <v>40</v>
       </c>
@@ -2860,7 +2857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="30">
+    <row r="27" spans="1:15" ht="15.6">
       <c r="A27" s="10" t="s">
         <v>22</v>
       </c>
@@ -2910,7 +2907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30">
+    <row r="28" spans="1:15" ht="15.6">
       <c r="A28" s="6" t="s">
         <v>100</v>
       </c>
@@ -2960,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30">
+    <row r="29" spans="1:15" ht="15.6">
       <c r="A29" s="6" t="s">
         <v>96</v>
       </c>
@@ -3010,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="30">
+    <row r="30" spans="1:15" ht="15.6">
       <c r="A30" s="10" t="s">
         <v>16</v>
       </c>
@@ -3060,7 +3057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30">
+    <row r="31" spans="1:15" ht="15.6">
       <c r="A31" s="6" t="s">
         <v>38</v>
       </c>
@@ -3110,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30">
+    <row r="32" spans="1:15" ht="15.6">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -3160,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="30">
+    <row r="33" spans="1:15" ht="15.6">
       <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
@@ -3210,7 +3207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="30">
+    <row r="34" spans="1:15" ht="15.6">
       <c r="A34" s="10" t="s">
         <v>18</v>
       </c>
@@ -3260,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="30">
+    <row r="35" spans="1:15" ht="15.6">
       <c r="A35" s="10" t="s">
         <v>109</v>
       </c>
@@ -3310,7 +3307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="30">
+    <row r="36" spans="1:15" ht="15.6">
       <c r="A36" s="6" t="s">
         <v>98</v>
       </c>
@@ -3360,7 +3357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="30">
+    <row r="37" spans="1:15" ht="15.6">
       <c r="A37" s="6" t="s">
         <v>103</v>
       </c>
@@ -3410,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30">
+    <row r="38" spans="1:15" ht="15.6">
       <c r="A38" s="10" t="s">
         <v>20</v>
       </c>
@@ -3460,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="30">
+    <row r="39" spans="1:15" ht="15.6">
       <c r="A39" s="10" t="s">
         <v>14</v>
       </c>
@@ -3510,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="30">
+    <row r="40" spans="1:15" ht="15.6">
       <c r="A40" s="10" t="s">
         <v>25</v>
       </c>
@@ -3560,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="30">
+    <row r="41" spans="1:15" ht="15.6">
       <c r="A41" s="6" t="s">
         <v>102</v>
       </c>
@@ -3610,7 +3607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="30">
+    <row r="42" spans="1:15" ht="15.6">
       <c r="A42" s="10" t="s">
         <v>24</v>
       </c>
@@ -3660,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="30">
+    <row r="43" spans="1:15" ht="15.6">
       <c r="A43" s="6" t="s">
         <v>93</v>
       </c>
@@ -3710,7 +3707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="30">
+    <row r="44" spans="1:15" ht="15.6">
       <c r="A44" s="6" t="s">
         <v>97</v>
       </c>
@@ -3760,7 +3757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30">
+    <row r="45" spans="1:15" ht="15.6">
       <c r="A45" s="6" t="s">
         <v>101</v>
       </c>
@@ -3810,7 +3807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30">
+    <row r="46" spans="1:15" ht="15.6">
       <c r="A46" s="6" t="s">
         <v>34</v>
       </c>
@@ -3860,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="30">
+    <row r="47" spans="1:15" ht="15.6">
       <c r="A47" s="6" t="s">
         <v>35</v>
       </c>
@@ -3910,7 +3907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="30">
+    <row r="48" spans="1:15" ht="15.6">
       <c r="A48" s="6" t="s">
         <v>99</v>
       </c>
@@ -3960,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="30">
+    <row r="49" spans="1:15" ht="15.6">
       <c r="A49" s="10" t="s">
         <v>23</v>
       </c>
@@ -4010,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="30">
+    <row r="50" spans="1:15" ht="15.6">
       <c r="A50" s="10" t="s">
         <v>110</v>
       </c>
@@ -4060,7 +4057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="30">
+    <row r="51" spans="1:15" ht="15.6">
       <c r="A51" s="6" t="s">
         <v>215</v>
       </c>
@@ -4110,7 +4107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="30">
+    <row r="52" spans="1:15" ht="15.6">
       <c r="A52" s="6" t="s">
         <v>235</v>
       </c>
@@ -4160,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="30">
+    <row r="53" spans="1:15" ht="15.6">
       <c r="A53" s="10" t="s">
         <v>206</v>
       </c>
@@ -4210,7 +4207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="30">
+    <row r="54" spans="1:15" ht="15.6">
       <c r="A54" s="6" t="s">
         <v>214</v>
       </c>
@@ -4260,7 +4257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="30">
+    <row r="55" spans="1:15" ht="15.6">
       <c r="A55" s="6" t="s">
         <v>213</v>
       </c>
@@ -4310,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="30">
+    <row r="56" spans="1:15" ht="15.6">
       <c r="A56" s="10" t="s">
         <v>202</v>
       </c>
@@ -4360,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="30">
+    <row r="57" spans="1:15" ht="15.6">
       <c r="A57" s="10" t="s">
         <v>234</v>
       </c>
@@ -4410,7 +4407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="30">
+    <row r="58" spans="1:15" ht="15.6">
       <c r="A58" s="6" t="s">
         <v>230</v>
       </c>
@@ -4460,7 +4457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="30">
+    <row r="59" spans="1:15" ht="15.6">
       <c r="A59" s="9" t="s">
         <v>217</v>
       </c>
@@ -4510,7 +4507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="30">
+    <row r="60" spans="1:15" ht="15.6">
       <c r="A60" s="9" t="s">
         <v>216</v>
       </c>
@@ -4560,7 +4557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="30">
+    <row r="61" spans="1:15" ht="15.6">
       <c r="A61" s="6" t="s">
         <v>219</v>
       </c>
@@ -4610,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="30">
+    <row r="62" spans="1:15" ht="15.6">
       <c r="A62" s="6" t="s">
         <v>218</v>
       </c>
@@ -4660,7 +4657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="30">
+    <row r="63" spans="1:15" ht="15.6">
       <c r="A63" s="10" t="s">
         <v>203</v>
       </c>
@@ -4710,7 +4707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="30">
+    <row r="64" spans="1:15" ht="15.6">
       <c r="A64" s="10" t="s">
         <v>240</v>
       </c>
@@ -4760,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="30">
+    <row r="65" spans="1:15" ht="15.6">
       <c r="A65" s="6" t="s">
         <v>221</v>
       </c>
@@ -4810,7 +4807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="30">
+    <row r="66" spans="1:15" ht="15.6">
       <c r="A66" s="6" t="s">
         <v>236</v>
       </c>
@@ -4860,7 +4857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="30">
+    <row r="67" spans="1:15" ht="15.6">
       <c r="A67" s="6" t="s">
         <v>4</v>
       </c>
@@ -4910,7 +4907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="30">
+    <row r="68" spans="1:15" ht="15.6">
       <c r="A68" s="6" t="s">
         <v>231</v>
       </c>
@@ -4960,7 +4957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="30">
+    <row r="69" spans="1:15" ht="15.6">
       <c r="A69" s="6" t="s">
         <v>222</v>
       </c>
@@ -5010,7 +5007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="30">
+    <row r="70" spans="1:15" ht="15.6">
       <c r="A70" s="6" t="s">
         <v>212</v>
       </c>
@@ -5060,7 +5057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="30">
+    <row r="71" spans="1:15" ht="15.6">
       <c r="A71" s="6" t="s">
         <v>232</v>
       </c>
@@ -5110,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="30">
+    <row r="72" spans="1:15" ht="15.6">
       <c r="A72" s="10" t="s">
         <v>205</v>
       </c>
@@ -5160,7 +5157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="30">
+    <row r="73" spans="1:15" ht="15.6">
       <c r="A73" s="10" t="s">
         <v>209</v>
       </c>
@@ -5210,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="30">
+    <row r="74" spans="1:15" ht="15.6">
       <c r="A74" s="10" t="s">
         <v>207</v>
       </c>
@@ -5260,7 +5257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="30">
+    <row r="75" spans="1:15" ht="15.6">
       <c r="A75" s="10" t="s">
         <v>207</v>
       </c>
@@ -5310,7 +5307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="30">
+    <row r="76" spans="1:15" ht="15.6">
       <c r="A76" s="10" t="s">
         <v>204</v>
       </c>
@@ -5360,7 +5357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="30">
+    <row r="77" spans="1:15" ht="15.6">
       <c r="A77" s="6" t="s">
         <v>233</v>
       </c>
@@ -5410,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="30">
+    <row r="78" spans="1:15" ht="15.6">
       <c r="A78" s="6" t="s">
         <v>238</v>
       </c>
@@ -5460,7 +5457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="30">
+    <row r="79" spans="1:15" ht="15.6">
       <c r="A79" s="6" t="s">
         <v>227</v>
       </c>
@@ -5510,7 +5507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="30">
+    <row r="80" spans="1:15" ht="15.6">
       <c r="A80" s="6" t="s">
         <v>224</v>
       </c>
@@ -5560,7 +5557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="30">
+    <row r="81" spans="1:15" ht="15.6">
       <c r="A81" s="10" t="s">
         <v>201</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="30">
+    <row r="82" spans="1:15" ht="15.6">
       <c r="A82" s="6" t="s">
         <v>228</v>
       </c>
@@ -5660,7 +5657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="30">
+    <row r="83" spans="1:15" ht="15.6">
       <c r="A83" s="6" t="s">
         <v>237</v>
       </c>
@@ -5710,7 +5707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="30">
+    <row r="84" spans="1:15" ht="15.6">
       <c r="A84" s="10" t="s">
         <v>200</v>
       </c>
@@ -5760,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="30">
+    <row r="85" spans="1:15" ht="15.6">
       <c r="A85" s="10" t="s">
         <v>241</v>
       </c>
@@ -5810,7 +5807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="30">
+    <row r="86" spans="1:15" ht="15.6">
       <c r="A86" s="6" t="s">
         <v>223</v>
       </c>
@@ -5860,7 +5857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="30">
+    <row r="87" spans="1:15" ht="15.6">
       <c r="A87" s="10" t="s">
         <v>208</v>
       </c>
@@ -5910,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="30">
+    <row r="88" spans="1:15" ht="15.6">
       <c r="A88" s="6" t="s">
         <v>229</v>
       </c>
@@ -5960,7 +5957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="30">
+    <row r="89" spans="1:15" ht="15.6">
       <c r="A89" s="6" t="s">
         <v>220</v>
       </c>
@@ -6010,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="30">
+    <row r="90" spans="1:15" ht="15.6">
       <c r="A90" s="10" t="s">
         <v>210</v>
       </c>
@@ -6060,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="30">
+    <row r="91" spans="1:15" ht="15.6">
       <c r="A91" s="6" t="s">
         <v>226</v>
       </c>
@@ -6110,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="30">
+    <row r="92" spans="1:15" ht="15.6">
       <c r="A92" s="6" t="s">
         <v>225</v>
       </c>
@@ -6160,7 +6157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="30">
+    <row r="93" spans="1:15" ht="15.6">
       <c r="A93" s="10" t="s">
         <v>239</v>
       </c>
@@ -6210,7 +6207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="30">
+    <row r="94" spans="1:15" ht="15.6">
       <c r="A94" s="6" t="s">
         <v>211</v>
       </c>
@@ -6260,7 +6257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="30">
+    <row r="95" spans="1:15" ht="15.6">
       <c r="A95" s="10" t="s">
         <v>247</v>
       </c>
@@ -6310,7 +6307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="30">
+    <row r="96" spans="1:15" ht="15.6">
       <c r="A96" s="10" t="s">
         <v>284</v>
       </c>
@@ -6360,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="30">
+    <row r="97" spans="1:15" ht="15.6">
       <c r="A97" s="6" t="s">
         <v>257</v>
       </c>
@@ -6410,7 +6407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="30">
+    <row r="98" spans="1:15" ht="15.6">
       <c r="A98" s="6" t="s">
         <v>272</v>
       </c>
@@ -6460,7 +6457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="30">
+    <row r="99" spans="1:15" ht="15.6">
       <c r="A99" s="6" t="s">
         <v>268</v>
       </c>
@@ -6510,7 +6507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="30">
+    <row r="100" spans="1:15" ht="15.6">
       <c r="A100" s="6" t="s">
         <v>276</v>
       </c>
@@ -6560,7 +6557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="30">
+    <row r="101" spans="1:15" ht="15.6">
       <c r="A101" s="10" t="s">
         <v>242</v>
       </c>
@@ -6610,7 +6607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="30">
+    <row r="102" spans="1:15" ht="15.6">
       <c r="A102" s="6" t="s">
         <v>278</v>
       </c>
@@ -6660,7 +6657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="30">
+    <row r="103" spans="1:15" ht="15.6">
       <c r="A103" s="8" t="s">
         <v>282</v>
       </c>
@@ -6710,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="30">
+    <row r="104" spans="1:15" ht="15.6">
       <c r="A104" s="6" t="s">
         <v>259</v>
       </c>
@@ -6760,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="30">
+    <row r="105" spans="1:15" ht="15.6">
       <c r="A105" s="6" t="s">
         <v>262</v>
       </c>
@@ -6810,7 +6807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="30">
+    <row r="106" spans="1:15" ht="15.6">
       <c r="A106" s="10" t="s">
         <v>283</v>
       </c>
@@ -6860,7 +6857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="30">
+    <row r="107" spans="1:15" ht="15.6">
       <c r="A107" s="6" t="s">
         <v>336</v>
       </c>
@@ -6910,7 +6907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="30">
+    <row r="108" spans="1:15" ht="15.6">
       <c r="A108" s="8" t="s">
         <v>280</v>
       </c>
@@ -6960,7 +6957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="30">
+    <row r="109" spans="1:15" ht="15.6">
       <c r="A109" s="6" t="s">
         <v>275</v>
       </c>
@@ -7010,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="30">
+    <row r="110" spans="1:15" ht="15.6">
       <c r="A110" s="6" t="s">
         <v>274</v>
       </c>
@@ -7060,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="30">
+    <row r="111" spans="1:15" ht="15.6">
       <c r="A111" s="10" t="s">
         <v>245</v>
       </c>
@@ -7110,7 +7107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="30">
+    <row r="112" spans="1:15" ht="15.6">
       <c r="A112" s="6" t="s">
         <v>255</v>
       </c>
@@ -7160,7 +7157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="30">
+    <row r="113" spans="1:17" ht="15.6">
       <c r="A113" s="6" t="s">
         <v>270</v>
       </c>
@@ -7210,7 +7207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="30">
+    <row r="114" spans="1:17" ht="15.6">
       <c r="A114" s="6" t="s">
         <v>265</v>
       </c>
@@ -7260,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="30">
+    <row r="115" spans="1:17" ht="15.6">
       <c r="A115" s="6" t="s">
         <v>267</v>
       </c>
@@ -7310,7 +7307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" ht="30">
+    <row r="116" spans="1:17" ht="15.6">
       <c r="A116" s="6" t="s">
         <v>260</v>
       </c>
@@ -7360,7 +7357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" ht="30">
+    <row r="117" spans="1:17" ht="15.6">
       <c r="A117" s="6" t="s">
         <v>273</v>
       </c>
@@ -7410,7 +7407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="30">
+    <row r="118" spans="1:17" ht="15.6">
       <c r="A118" s="10" t="s">
         <v>249</v>
       </c>
@@ -7460,7 +7457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="30">
+    <row r="119" spans="1:17" ht="15.6">
       <c r="A119" s="6" t="s">
         <v>261</v>
       </c>
@@ -7510,7 +7507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="30">
+    <row r="120" spans="1:17" ht="15.6">
       <c r="A120" s="6" t="s">
         <v>277</v>
       </c>
@@ -7560,7 +7557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="30">
+    <row r="121" spans="1:17" ht="15.6">
       <c r="A121" s="10" t="s">
         <v>250</v>
       </c>
@@ -7610,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="30">
+    <row r="122" spans="1:17" ht="15.6">
       <c r="A122" s="8" t="s">
         <v>281</v>
       </c>
@@ -7660,7 +7657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="30">
+    <row r="123" spans="1:17" ht="15.6">
       <c r="A123" s="10" t="s">
         <v>244</v>
       </c>
@@ -7710,7 +7707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="30">
+    <row r="124" spans="1:17" ht="15.6">
       <c r="A124" s="10" t="s">
         <v>13</v>
       </c>
@@ -7761,7 +7758,7 @@
       </c>
       <c r="Q124" s="5"/>
     </row>
-    <row r="125" spans="1:17" ht="30">
+    <row r="125" spans="1:17" ht="15.6">
       <c r="A125" s="6" t="s">
         <v>264</v>
       </c>
@@ -7811,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:17" ht="30">
+    <row r="126" spans="1:17" ht="15.6">
       <c r="A126" s="10" t="s">
         <v>251</v>
       </c>
@@ -7861,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="30">
+    <row r="127" spans="1:17" ht="15.6">
       <c r="A127" s="10" t="s">
         <v>248</v>
       </c>
@@ -7911,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="30">
+    <row r="128" spans="1:17" ht="15.6">
       <c r="A128" s="10" t="s">
         <v>246</v>
       </c>
@@ -7961,7 +7958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="30">
+    <row r="129" spans="1:15" ht="15.6">
       <c r="A129" s="6" t="s">
         <v>254</v>
       </c>
@@ -8011,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="30">
+    <row r="130" spans="1:15" ht="15.6">
       <c r="A130" s="10" t="s">
         <v>252</v>
       </c>
@@ -8061,7 +8058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="30">
+    <row r="131" spans="1:15" ht="15.6">
       <c r="A131" s="6" t="s">
         <v>258</v>
       </c>
@@ -8111,7 +8108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="30">
+    <row r="132" spans="1:15" ht="15.6">
       <c r="A132" s="6" t="s">
         <v>263</v>
       </c>
@@ -8161,7 +8158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="30">
+    <row r="133" spans="1:15" ht="15.6">
       <c r="A133" s="6" t="s">
         <v>266</v>
       </c>
@@ -8211,7 +8208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="30">
+    <row r="134" spans="1:15" ht="15.6">
       <c r="A134" s="10" t="s">
         <v>243</v>
       </c>
@@ -8261,7 +8258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="30">
+    <row r="135" spans="1:15" ht="15.6">
       <c r="A135" s="6" t="s">
         <v>256</v>
       </c>
@@ -8311,7 +8308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="30">
+    <row r="136" spans="1:15" ht="15.6">
       <c r="A136" s="6" t="s">
         <v>269</v>
       </c>
@@ -8361,7 +8358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="30">
+    <row r="137" spans="1:15" ht="15.6">
       <c r="A137" s="6" t="s">
         <v>279</v>
       </c>
@@ -8411,7 +8408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="30">
+    <row r="138" spans="1:15" ht="15.6">
       <c r="A138" s="9" t="s">
         <v>253</v>
       </c>
@@ -8461,7 +8458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="30">
+    <row r="139" spans="1:15" ht="15.6">
       <c r="A139" s="6" t="s">
         <v>271</v>
       </c>
@@ -8511,7 +8508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="30">
+    <row r="140" spans="1:15" ht="15.6">
       <c r="A140" s="6" t="s">
         <v>325</v>
       </c>
@@ -8561,7 +8558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="30">
+    <row r="141" spans="1:15" ht="15.6">
       <c r="A141" s="6" t="s">
         <v>318</v>
       </c>
@@ -8611,7 +8608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="30">
+    <row r="142" spans="1:15" ht="15.6">
       <c r="A142" s="10" t="s">
         <v>333</v>
       </c>
@@ -8661,7 +8658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="30">
+    <row r="143" spans="1:15" ht="15.6">
       <c r="A143" s="6" t="s">
         <v>340</v>
       </c>
@@ -8711,7 +8708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="30">
+    <row r="144" spans="1:15" ht="15.6">
       <c r="A144" s="10" t="s">
         <v>330</v>
       </c>
@@ -8761,7 +8758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="30">
+    <row r="145" spans="1:15" ht="15.6">
       <c r="A145" s="6" t="s">
         <v>319</v>
       </c>
@@ -8811,7 +8808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="30">
+    <row r="146" spans="1:15" ht="15.6">
       <c r="A146" s="6" t="s">
         <v>327</v>
       </c>
@@ -8861,7 +8858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="30">
+    <row r="147" spans="1:15" ht="15.6">
       <c r="A147" s="6" t="s">
         <v>326</v>
       </c>
@@ -8911,7 +8908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="30">
+    <row r="148" spans="1:15" ht="15.6">
       <c r="A148" s="10" t="s">
         <v>332</v>
       </c>
@@ -8961,7 +8958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="30">
+    <row r="149" spans="1:15" ht="15.6">
       <c r="A149" s="10" t="s">
         <v>331</v>
       </c>
@@ -9011,7 +9008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="30">
+    <row r="150" spans="1:15" ht="15.6">
       <c r="A150" s="10" t="s">
         <v>313</v>
       </c>
@@ -9061,7 +9058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="30">
+    <row r="151" spans="1:15" ht="15.6">
       <c r="A151" s="10" t="s">
         <v>334</v>
       </c>
@@ -9111,7 +9108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="30">
+    <row r="152" spans="1:15" ht="15.6">
       <c r="A152" s="6" t="s">
         <v>338</v>
       </c>
@@ -9161,7 +9158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="30">
+    <row r="153" spans="1:15" ht="15.6">
       <c r="A153" s="6" t="s">
         <v>337</v>
       </c>
@@ -9211,7 +9208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="30">
+    <row r="154" spans="1:15" ht="15.6">
       <c r="A154" s="6" t="s">
         <v>324</v>
       </c>
@@ -9261,7 +9258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="30">
+    <row r="155" spans="1:15" ht="15.6">
       <c r="A155" s="10" t="s">
         <v>316</v>
       </c>
@@ -9311,7 +9308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="30">
+    <row r="156" spans="1:15" ht="15.6">
       <c r="A156" s="6" t="s">
         <v>323</v>
       </c>
@@ -9361,7 +9358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="30">
+    <row r="157" spans="1:15" ht="15.6">
       <c r="A157" s="10" t="s">
         <v>329</v>
       </c>
@@ -9411,7 +9408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="30">
+    <row r="158" spans="1:15" ht="15.6">
       <c r="A158" s="6" t="s">
         <v>320</v>
       </c>
@@ -9461,7 +9458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="30">
+    <row r="159" spans="1:15" ht="15.6">
       <c r="A159" s="10" t="s">
         <v>312</v>
       </c>
@@ -9511,7 +9508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="30">
+    <row r="160" spans="1:15" ht="15.6">
       <c r="A160" s="9" t="s">
         <v>314</v>
       </c>
@@ -9561,7 +9558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="30">
+    <row r="161" spans="1:15" ht="15.6">
       <c r="A161" s="9" t="s">
         <v>328</v>
       </c>
@@ -9611,7 +9608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="30">
+    <row r="162" spans="1:15" ht="15.6">
       <c r="A162" s="10" t="s">
         <v>311</v>
       </c>
@@ -9661,7 +9658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="30">
+    <row r="163" spans="1:15" ht="15.6">
       <c r="A163" s="6" t="s">
         <v>317</v>
       </c>
@@ -9711,7 +9708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="30">
+    <row r="164" spans="1:15" ht="15.6">
       <c r="A164" s="10" t="s">
         <v>322</v>
       </c>
@@ -9761,7 +9758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="30">
+    <row r="165" spans="1:15" ht="15.6">
       <c r="A165" s="6" t="s">
         <v>321</v>
       </c>
@@ -9811,7 +9808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="30">
+    <row r="166" spans="1:15" ht="15.6">
       <c r="A166" s="6" t="s">
         <v>315</v>
       </c>
@@ -9861,7 +9858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="30">
+    <row r="167" spans="1:15" ht="15">
       <c r="E167" s="8" t="s">
         <v>343</v>
       </c>
@@ -9874,7 +9871,7 @@
         <v>25</v>
       </c>
       <c r="H167" s="17">
-        <f t="shared" ref="H167:K167" si="16">COUNTIF(H2:H166,"Absent")</f>
+        <f t="shared" ref="H167:L167" si="16">COUNTIF(H2:H166,"Absent")</f>
         <v>93</v>
       </c>
       <c r="I167" s="17">
@@ -9889,7 +9886,10 @@
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="L167" s="18"/>
+      <c r="L167" s="17">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A140:O166">

</xml_diff>

<commit_message>
My attendance forgot to add
</commit_message>
<xml_diff>
--- a/attendance_data.xlsx
+++ b/attendance_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\attendance_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF99E4F4-077D-44BF-9B40-62599C2C63BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAA2947-4222-4209-952C-E7A44EBD0E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F33DA19-6151-4346-A3A3-5311E8A75F56}"/>
   </bookViews>
@@ -1522,9 +1522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778A1F93-BD03-4755-A395-19876E27A1C7}">
   <dimension ref="A1:S167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P165" sqref="P165"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="74" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L139" sqref="L139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9446,7 +9446,7 @@
         <v>89</v>
       </c>
       <c r="N139" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O139" s="9">
         <v>5</v>
@@ -11038,7 +11038,7 @@
       </c>
       <c r="N167" s="16">
         <f t="shared" si="16"/>
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>